<commit_message>
Hibák amit Krisztián talált az javítva
</commit_message>
<xml_diff>
--- a/Tesztelés/App-teszt/Applikáció-teszt.xlsx
+++ b/Tesztelés/App-teszt/Applikáció-teszt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\terkerter\Tesztelés\App-teszt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TeruletKeruletTerfogat\Tesztelés\App-teszt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="58">
   <si>
     <t>Sorszám</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>r sugárhoz 0át írok be</t>
+  </si>
+  <si>
+    <t>Javítva</t>
   </si>
 </sst>
 </file>
@@ -645,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +663,7 @@
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -680,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -700,7 +703,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -720,7 +723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -740,7 +743,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -760,7 +763,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -780,7 +783,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -800,7 +803,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -820,7 +823,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -840,7 +843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -860,7 +863,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -879,8 +882,11 @@
       <c r="F11" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -899,8 +905,11 @@
       <c r="F12" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -919,8 +928,11 @@
       <c r="F13" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G13" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -939,8 +951,11 @@
       <c r="F14" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -959,8 +974,11 @@
       <c r="F15" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -979,8 +997,11 @@
       <c r="F16" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -999,8 +1020,11 @@
       <c r="F17" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1019,8 +1043,11 @@
       <c r="F18" s="15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1039,8 +1066,11 @@
       <c r="F19" s="16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1060,7 +1090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1080,7 +1110,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1100,7 +1130,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1120,7 +1150,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1140,7 +1170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1160,7 +1190,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1180,7 +1210,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1200,7 +1230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1220,7 +1250,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1240,7 +1270,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1260,7 +1290,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1280,7 +1310,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>

</xml_diff>